<commit_message>
final files from john
</commit_message>
<xml_diff>
--- a/DATA/presidents.xlsx
+++ b/DATA/presidents.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="US Presidents" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="280">
   <si>
     <t>Term</t>
   </si>
@@ -840,22 +840,39 @@
   </si>
   <si>
     <t>Hawaii</t>
+  </si>
+  <si>
+    <t>2017-01-20</t>
+  </si>
+  <si>
+    <t>Trump</t>
+  </si>
+  <si>
+    <t>Donald J</t>
+  </si>
+  <si>
+    <t>1946-06-14</t>
+  </si>
+  <si>
+    <t>Queens, NYC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="MM/DD/YY"/>
+    <numFmt numFmtId="167" formatCode="MM/DD/YYYY"/>
   </numFmts>
   <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -915,7 +932,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -925,6 +942,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -943,27 +964,27 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J45"/>
+  <dimension ref="A1:J46"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C24" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C45" activeCellId="0" sqref="C45"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A24" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D47" activeCellId="0" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="5.85204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.3724489795918"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.6836734693878"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="10.6938775510204"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.4183673469388"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.3928571428571"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.0663265306122"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.9387755102041"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="21.1683673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.19897959183674"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.4795918367347"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.5765306122449"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="29.8775510204082"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.9183673469388"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.6377551020408"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.3775510204082"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="26.8163265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="14.5816326530612"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2364,7 +2385,7 @@
       <c r="G44" s="0" t="s">
         <v>268</v>
       </c>
-      <c r="H44" s="2" t="s">
+      <c r="H44" s="3" t="s">
         <v>264</v>
       </c>
       <c r="I44" s="2" t="s">
@@ -2400,10 +2421,42 @@
         <v>269</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>243</v>
+        <v>275</v>
       </c>
       <c r="J45" s="0" t="s">
         <v>54</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>276</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>277</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="E46" s="0" t="s">
+        <v>243</v>
+      </c>
+      <c r="F46" s="0" t="s">
+        <v>279</v>
+      </c>
+      <c r="G46" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="I46" s="0" t="s">
+        <v>243</v>
+      </c>
+      <c r="J46" s="0" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>